<commit_message>
continuing the overhaul of replacing the two impact & hazard objects with a single table
</commit_message>
<xml_diff>
--- a/Taxonomies/OOP_HazImp_DataDictionaries.xlsx
+++ b/Taxonomies/OOP_HazImp_DataDictionaries.xlsx
@@ -21,7 +21,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="148">
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
   <si>
     <t xml:space="preserve">Variable Name</t>
   </si>
@@ -32,6 +35,9 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">BASIC INFO</t>
+  </si>
+  <si>
     <t xml:space="preserve">GCDB_ID</t>
   </si>
   <si>
@@ -107,45 +113,16 @@
     <t xml:space="preserve">prim_haz_cluster</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Primary i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">mpacting hazard cluster</t>
-    </r>
+    <t xml:space="preserve">Primary impacting hazard cluster</t>
   </si>
   <si>
     <t xml:space="preserve">prim_haz_spec</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Primary i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">mpacting specific hazard</t>
-    </r>
+    <t xml:space="preserve">Primary impacting specific hazard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPACT</t>
   </si>
   <si>
     <t xml:space="preserve">impsub_ID</t>
@@ -214,94 +191,33 @@
     <t xml:space="preserve">Estimate type: primary  secondary modelled</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">imp_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">src_db</t>
-    </r>
+    <t xml:space="preserve">imp_src_db</t>
   </si>
   <si>
     <t xml:space="preserve">Source database name of impact estimate or the curated estimate</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">imp_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">src_org</t>
-    </r>
+    <t xml:space="preserve">imp_src_org</t>
   </si>
   <si>
     <t xml:space="preserve">Source organisation of impact estimate or the curated estimate</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">imp_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">src_orgtype</t>
-    </r>
+    <t xml:space="preserve">imp_src_orgtype</t>
   </si>
   <si>
     <t xml:space="preserve">Source organisation type</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">imp_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">src_URL</t>
-    </r>
+    <t xml:space="preserve">imp_src_URL</t>
   </si>
   <si>
     <t xml:space="preserve">URL of the impact estimate</t>
   </si>
   <si>
+    <t xml:space="preserve">HAZARD</t>
+  </si>
+  <si>
     <t xml:space="preserve">subhaz_ID</t>
   </si>
   <si>
@@ -311,156 +227,31 @@
     <t xml:space="preserve">haz_Ab</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">haz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">type</t>
-    </r>
+    <t xml:space="preserve">haz_type</t>
   </si>
   <si>
     <t xml:space="preserve">Impacting hazard type</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">haz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">cluster</t>
-    </r>
+    <t xml:space="preserve">haz_cluster</t>
   </si>
   <si>
     <t xml:space="preserve">Impacting hazard cluster</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">haz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">spec</t>
-    </r>
+    <t xml:space="preserve">haz_spec</t>
   </si>
   <si>
     <t xml:space="preserve">Impacting specific hazard</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">haz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">link</t>
-    </r>
+    <t xml:space="preserve">haz_link</t>
   </si>
   <si>
     <t xml:space="preserve">Associated impactful-hazards to the specific hazard</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">haz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">potlink</t>
-    </r>
+    <t xml:space="preserve">haz_potlink</t>
   </si>
   <si>
     <t xml:space="preserve">Potential other impactful-hazards that may be associated to the specific hazard</t>
@@ -481,6 +272,9 @@
     <t xml:space="preserve">haz_src_URL</t>
   </si>
   <si>
+    <t xml:space="preserve">SPATIAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">imp_spat_ID</t>
   </si>
   <si>
@@ -508,61 +302,13 @@
     <t xml:space="preserve">haz_spat_ID</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">haz_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">spat_type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">haz_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">spat_res</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">haz_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">spat_srcorg</t>
-    </r>
+    <t xml:space="preserve">haz_spat_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haz_spat_res</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haz_spat_srcorg</t>
   </si>
   <si>
     <t xml:space="preserve">GLIDE number of hazard (not necessarily the primary hazard)</t>
@@ -728,7 +474,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -752,31 +498,106 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFE0EFD4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADC5E7"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDAA2"/>
+        <bgColor rgb="FFFCD4D1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EFD4"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD4D1"/>
+        <bgColor rgb="FFFFDAA2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -805,7 +626,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -814,7 +635,83 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -824,38 +721,99 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFCD4D1"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFE0EFD4"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFADC5E7"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFDAA2"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMK52"/>
+  <dimension ref="A1:AMJ49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="70.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="65.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -865,40 +823,47 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="A3" s="3"/>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="0"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -1919,19 +1884,18 @@
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
-      <c r="AMK4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="0"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -2952,496 +2916,551 @@
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
-      <c r="AMK5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
+      <c r="A7" s="3"/>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
+      <c r="A8" s="3"/>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
+      <c r="D10" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
+      <c r="A11" s="3"/>
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
+      <c r="B13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
+      <c r="B14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="B20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="B21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7"/>
+      <c r="B22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7"/>
+      <c r="B23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7"/>
+      <c r="B24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7"/>
+      <c r="B25" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7"/>
+      <c r="B26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="B27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7"/>
+      <c r="B28" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13"/>
+      <c r="B31" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13"/>
+      <c r="B32" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13"/>
+      <c r="B33" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13"/>
+      <c r="B34" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="13"/>
+      <c r="B35" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13"/>
+      <c r="B36" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13"/>
+      <c r="B37" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13"/>
+      <c r="B38" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="13"/>
+      <c r="B39" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13"/>
+      <c r="B40" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>58</v>
+      <c r="A42" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>60</v>
+      <c r="A43" s="17"/>
+      <c r="B43" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="17"/>
+      <c r="B44" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>80</v>
+      <c r="A45" s="17"/>
+      <c r="B45" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>82</v>
+      <c r="A46" s="17"/>
+      <c r="B46" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>84</v>
+      <c r="A47" s="17"/>
+      <c r="B47" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>86</v>
+      <c r="A48" s="17"/>
+      <c r="B48" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>86</v>
+      <c r="A49" s="17"/>
+      <c r="B49" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A15:A29"/>
+    <mergeCell ref="A30:A41"/>
+    <mergeCell ref="A42:A49"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3450,7 +3469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3460,423 +3479,423 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="22" t="s">
         <v>2</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>